<commit_message>
removing silly log files
</commit_message>
<xml_diff>
--- a/misc/hours.xlsx
+++ b/misc/hours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C657A96B-8BBF-427D-A9B8-E3AB2F54EACD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C68AA37-4910-44D3-B7D2-28D49DC9A816}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>locus questions</t>
+  </si>
+  <si>
+    <t>setting up github</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +465,17 @@
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
morning commute solution plus post draft
</commit_message>
<xml_diff>
--- a/misc/hours.xlsx
+++ b/misc/hours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C68AA37-4910-44D3-B7D2-28D49DC9A816}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38024B6E-B0AA-4372-ACE0-19BEC2AA9278}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>setting up github</t>
+  </si>
+  <si>
+    <t>worked solution; commute q.</t>
   </si>
 </sst>
 </file>
@@ -366,16 +369,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -414,66 +417,88 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>43311</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <v>0.6875</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>0.72916666666666663</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E5" si="0">C3-B3</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.99998842592592585</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2">
+        <f t="shared" ref="E4:E7" si="0">C4-B4</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.99998842592592585</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>0.16665509259259248</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>43315</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>43317</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>0.5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C7" s="2">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
+      </c>
+      <c r="E7" s="2">
+        <f>C7-B7</f>
+        <v>7.291666666666663E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2">
+        <f>C8-B8</f>
+        <v>0.13541666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>